<commit_message>
Auto commit and push all modified files
</commit_message>
<xml_diff>
--- a/analysis/frailty_matched_cohorts.xlsx
+++ b/analysis/frailty_matched_cohorts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stk\Documents\GitHub\Czech\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6D83D3-B2AF-463A-8A3F-BDEFCDA019E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C4BEFA-7627-43CE-84E4-06A1A82E95CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1965" windowWidth="22755" windowHeight="13860" xr2:uid="{9EE634CF-6E59-49B5-9852-F93E8D19BEDD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{9EE634CF-6E59-49B5-9852-F93E8D19BEDD}"/>
   </bookViews>
   <sheets>
     <sheet name="DEATH matched cohort" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="71">
   <si>
     <t>birth year</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>Under 80 cohort</t>
+  </si>
+  <si>
+    <t>Compute average age</t>
+  </si>
+  <si>
+    <t>The SIZES are matched, but deaths are not!!</t>
   </si>
 </sst>
 </file>
@@ -728,7 +734,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -747,6 +753,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -886,7 +893,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>) is actually the BEST evidence of lack of benefit bec ause the death counts match up during no COVID and COVID, but the frailty is still 1.8 hgiher for the unvaccinated</a:t>
+            <a:t>) is actually the BEST evidence of lack of benefit because the death counts match up during no COVID and COVID, but the frailty is still 1.8 hgiher for the unvaccinated</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1015,7 +1022,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>Better to use the DEATH MATCHED cohort with the 1.8x higher frailty for the unvaccinated.</a:t>
+            <a:t>Better to use the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>DEATH MATCHED </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>cohort with the 1.8x higher frailty for the unvaccinated.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -1095,7 +1110,15 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> cohort. But this cohort is YOUNGER and 26% LESS frail, so it could be attacked as "cheating".</a:t>
+            <a:t> cohort. But this cohort is YOUNGER and 26% LESS </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>frail per capita, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>but that's because we added a bunch of young people.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1103,10 +1126,12 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>The DEATH matched cohort is only slightly younger, but 1.8X more frail, so that cohort cannot be attacked as "cheating."</a:t>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>So using cohort size isn't a great way to assess frailty because adding people unlikely to die is misleaing.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1434,19 +1459,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D152082-2FE5-43E6-BD44-FFAC07E42B4D}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="31.1796875" customWidth="1"/>
+    <col min="9" max="9" width="25.26953125" customWidth="1"/>
+    <col min="10" max="10" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1506,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1507,7 +1532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1533,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1559,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1585,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1611,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1637,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1663,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1689,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1715,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1741,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1767,7 +1792,7 @@
         <v>7.58</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1793,7 +1818,7 @@
         <v>53.42</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1819,7 +1844,7 @@
         <v>64.290000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1845,7 +1870,7 @@
         <v>72.13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1871,7 +1896,7 @@
         <v>78.56</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1897,7 +1922,7 @@
         <v>82.19</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1923,7 +1948,7 @@
         <v>82.42</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1960,7 +1985,7 @@
         <v>8054475</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1997,7 +2022,7 @@
         <v>10377430</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2034,7 +2059,7 @@
         <v>11641435</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2071,7 +2096,7 @@
         <v>13890960</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2108,7 +2133,7 @@
         <v>15200625</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2145,7 +2170,7 @@
         <v>18392900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2182,7 +2207,7 @@
         <v>20374785</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2219,7 +2244,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2245,7 +2270,7 @@
         <v>31.78</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2274,7 +2299,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -2306,7 +2331,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -2338,7 +2363,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -2364,7 +2389,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -2392,7 +2417,7 @@
       <c r="L32" t="s">
         <v>50</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="8">
         <f>H36/I36</f>
         <v>1.8695747599762487</v>
       </c>
@@ -2400,7 +2425,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -2429,7 +2454,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2458,7 +2483,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -2478,7 +2503,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="G36" s="4" t="s">
         <v>43</v>
       </c>
@@ -2491,30 +2516,30 @@
         <v>1763263</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="O37" t="s">
+      <c r="O37" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O40" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O41" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O42" t="s">
         <v>59</v>
       </c>
@@ -2530,15 +2555,17 @@
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31:H31"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="30.90625" customWidth="1"/>
+    <col min="3" max="3" width="26.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2561,7 +2588,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
@@ -2575,7 +2602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -2589,7 +2616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -2603,7 +2630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
@@ -2617,7 +2644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -2631,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
@@ -2645,7 +2672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
@@ -2659,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
@@ -2673,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -2687,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -2701,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2715,7 +2742,7 @@
         <v>7.58</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
@@ -2729,7 +2756,7 @@
         <v>53.42</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -2743,7 +2770,7 @@
         <v>64.290000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
@@ -2757,7 +2784,7 @@
         <v>72.13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
@@ -2770,8 +2797,11 @@
       <c r="D16" s="5">
         <v>78.56</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
@@ -2785,7 +2815,7 @@
         <v>82.19</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
@@ -2805,7 +2835,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -2822,15 +2852,15 @@
         <v>75</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:H25" si="0">B19*$F19</f>
+        <f>B19*$F19</f>
         <v>35119125</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G19:H25" si="0">C19*$F19</f>
         <v>8054475</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>22</v>
       </c>
@@ -2855,7 +2885,7 @@
         <v>10377430</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
@@ -2880,7 +2910,7 @@
         <v>11641435</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -2905,7 +2935,7 @@
         <v>13890960</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -2930,7 +2960,7 @@
         <v>15200625</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>26</v>
       </c>
@@ -2955,7 +2985,7 @@
         <v>18392900</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>27</v>
       </c>
@@ -2980,7 +3010,7 @@
         <v>20374785</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>28</v>
       </c>
@@ -3008,7 +3038,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>29</v>
       </c>
@@ -3033,7 +3063,7 @@
         <v>17647070</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>30</v>
       </c>
@@ -3058,7 +3088,7 @@
         <v>16489650</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>31</v>
       </c>
@@ -3083,7 +3113,7 @@
         <v>10985400</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>32</v>
       </c>
@@ -3108,7 +3138,7 @@
         <v>9218320</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
@@ -3133,7 +3163,7 @@
         <v>40.85696231994951</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>34</v>
       </c>
@@ -3147,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
@@ -3161,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>36</v>
       </c>
@@ -3175,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>61</v>
       </c>
@@ -3190,27 +3220,30 @@
       <c r="G36" t="s">
         <v>50</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="8">
         <f>B36/C36</f>
         <v>0.99217820555138858</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>67</v>
       </c>
@@ -3225,19 +3258,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C7E18B-62CE-45A2-967F-CC757CFCF5B2}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="31.1796875" customWidth="1"/>
+    <col min="9" max="9" width="25.26953125" customWidth="1"/>
+    <col min="10" max="10" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3272,7 +3305,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3298,7 +3331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3324,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -3350,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -3376,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -3402,7 +3435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -3428,7 +3461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -3454,7 +3487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3480,7 +3513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -3506,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3532,7 +3565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -3558,7 +3591,7 @@
         <v>7.58</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -3584,7 +3617,7 @@
         <v>53.42</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -3610,7 +3643,7 @@
         <v>64.290000000000006</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -3636,7 +3669,7 @@
         <v>72.13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -3662,7 +3695,7 @@
         <v>78.56</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -3688,7 +3721,7 @@
         <v>82.19</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -3725,7 +3758,7 @@
         <v>5315440</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -3762,7 +3795,7 @@
         <v>8054475</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -3799,7 +3832,7 @@
         <v>10377430</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -3836,7 +3869,7 @@
         <v>11641435</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -3873,7 +3906,7 @@
         <v>13890960</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -3910,7 +3943,7 @@
         <v>15200625</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -3947,7 +3980,7 @@
         <v>18392900</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -3984,7 +4017,7 @@
         <v>20374785</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -4024,7 +4057,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -4061,7 +4094,7 @@
         <v>17647070</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -4098,7 +4131,7 @@
         <v>16489650</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -4135,7 +4168,7 @@
         <v>10985400</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -4172,7 +4205,7 @@
         <v>9218320</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -4209,7 +4242,7 @@
         <v>8778840</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -4246,7 +4279,7 @@
         <v>5600320</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -4283,7 +4316,7 @@
         <v>2361640</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -4320,7 +4353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -4345,7 +4378,7 @@
         <v>31.980088438605243</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="G36" s="4" t="s">
         <v>68</v>
       </c>
@@ -4358,7 +4391,7 @@
         <v>6019317</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -4366,7 +4399,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L38" t="s">
         <v>48</v>
       </c>
@@ -4374,7 +4407,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L39" t="s">
         <v>49</v>
       </c>
@@ -4382,7 +4415,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="L41" t="s">
         <v>50</v>
       </c>

</xml_diff>